<commit_message>
Actualización del Cronograma - Modificación del % de avance
</commit_message>
<xml_diff>
--- a/lineas_base/FRSIAAATR/LB_Planificacion/FRSIAAATR_C.xlsx
+++ b/lineas_base/FRSIAAATR/LB_Planificacion/FRSIAAATR_C.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Plan de proyecto y Gantt" sheetId="1" r:id="rId1"/>
     <sheet name="Línea base de costo" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1332,6 +1332,27 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1341,6 +1362,102 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1352,123 +1469,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2167,7 +2167,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000017-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{00000018-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2177,7 +2177,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000018-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{00000019-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2187,7 +2187,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000019-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{0000001A-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2197,7 +2197,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000001A-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{0000001B-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2207,7 +2207,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000001B-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{0000001C-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2217,7 +2217,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000001C-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{0000001D-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2227,7 +2227,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000001D-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{0000001E-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2237,7 +2237,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000001E-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{0000001F-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2247,7 +2247,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000001F-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{00000020-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2257,7 +2257,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000020-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{00000021-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2267,7 +2267,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000021-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{00000022-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2277,7 +2277,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000022-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{00000023-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2287,7 +2287,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000023-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{00000024-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2297,7 +2297,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000024-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{00000025-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2307,7 +2307,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000025-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{00000026-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2317,7 +2317,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000026-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{00000027-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2327,7 +2327,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000027-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{00000028-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2337,7 +2337,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000028-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{00000029-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2347,7 +2347,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000029-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{0000002A-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2357,7 +2357,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000002A-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{0000002B-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2367,7 +2367,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000002B-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{0000002C-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2377,7 +2377,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000002C-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{0000002D-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2387,7 +2387,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000002D-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{0000002E-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2397,7 +2397,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000002E-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{0000002F-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2407,7 +2407,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000002F-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{00000030-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2417,7 +2417,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000030-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{00000031-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2427,7 +2427,7 @@
             <c:bubble3D val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000031-BC27-42F0-95D7-3BD26C201260}"/>
+                <c16:uniqueId val="{00000032-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2435,11 +2435,6 @@
             <c:idx val="79"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000032-BC27-42F0-95D7-3BD26C201260}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="80"/>
@@ -2835,11 +2830,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="277669520"/>
-        <c:axId val="277667888"/>
+        <c:axId val="-1037065632"/>
+        <c:axId val="-1037064000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="277669520"/>
+        <c:axId val="-1037065632"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2882,7 +2877,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277667888"/>
+        <c:crossAx val="-1037064000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2890,7 +2885,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="277667888"/>
+        <c:axId val="-1037064000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="44078"/>
@@ -2943,7 +2938,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277669520"/>
+        <c:crossAx val="-1037065632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="15"/>
@@ -3558,7 +3553,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3903,8 +3898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3927,21 +3922,21 @@
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
-      <c r="J2" s="137"/>
-      <c r="K2" s="137"/>
-      <c r="L2" s="137"/>
-      <c r="M2" s="137"/>
-      <c r="N2" s="137"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="94"/>
+      <c r="M2" s="94"/>
+      <c r="N2" s="94"/>
       <c r="O2" s="25"/>
       <c r="P2" s="25"/>
       <c r="Q2" s="25"/>
@@ -3955,15 +3950,15 @@
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="138" t="s">
+      <c r="B3" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="138"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
@@ -3983,15 +3978,15 @@
       <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="138" t="s">
+      <c r="B4" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="138"/>
-      <c r="D4" s="138"/>
-      <c r="E4" s="138"/>
-      <c r="F4" s="138"/>
-      <c r="G4" s="138"/>
-      <c r="H4" s="138"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="95"/>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
@@ -4011,15 +4006,15 @@
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="139" t="s">
+      <c r="B5" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="139"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
@@ -4120,7 +4115,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="5">
-        <v>0.43</v>
+        <v>0.46</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -4269,7 +4264,7 @@
       <c r="C13" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="105"/>
+      <c r="D13" s="130"/>
       <c r="E13" s="26"/>
       <c r="F13" s="26" t="s">
         <v>26</v>
@@ -4305,16 +4300,16 @@
       <c r="V13" s="25"/>
     </row>
     <row r="14" spans="1:22" s="25" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A14" s="114" t="s">
+      <c r="A14" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="110" t="s">
+      <c r="B14" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="116" t="s">
+      <c r="C14" s="107" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="106"/>
+      <c r="D14" s="131"/>
       <c r="E14" s="90" t="s">
         <v>31</v>
       </c>
@@ -4342,10 +4337,10 @@
       </c>
     </row>
     <row r="15" spans="1:22" s="25" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A15" s="115"/>
-      <c r="B15" s="112"/>
-      <c r="C15" s="117"/>
-      <c r="D15" s="106"/>
+      <c r="A15" s="123"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="125"/>
+      <c r="D15" s="131"/>
       <c r="E15" s="90" t="s">
         <v>31</v>
       </c>
@@ -4382,7 +4377,7 @@
       <c r="C16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="106"/>
+      <c r="D16" s="131"/>
       <c r="E16" s="43" t="s">
         <v>34</v>
       </c>
@@ -4418,7 +4413,7 @@
       <c r="C17" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="107"/>
+      <c r="D17" s="132"/>
       <c r="E17" s="44" t="s">
         <v>36</v>
       </c>
@@ -4449,12 +4444,12 @@
       <c r="A18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="98"/>
-      <c r="C18" s="99"/>
-      <c r="D18" s="99"/>
-      <c r="E18" s="99"/>
-      <c r="F18" s="99"/>
-      <c r="G18" s="100"/>
+      <c r="B18" s="137"/>
+      <c r="C18" s="138"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="138"/>
+      <c r="F18" s="138"/>
+      <c r="G18" s="139"/>
       <c r="H18" s="27">
         <v>44008</v>
       </c>
@@ -4484,16 +4479,16 @@
       <c r="V18" s="25"/>
     </row>
     <row r="19" spans="1:22" s="25" customFormat="1" ht="36" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="123" t="s">
+      <c r="C19" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="94" t="s">
+      <c r="D19" s="101" t="s">
         <v>39</v>
       </c>
       <c r="E19" s="89" t="s">
@@ -4522,10 +4517,10 @@
       </c>
     </row>
     <row r="20" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="102"/>
-      <c r="B20" s="95"/>
-      <c r="C20" s="124"/>
-      <c r="D20" s="95"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="102"/>
+      <c r="C20" s="105"/>
+      <c r="D20" s="102"/>
       <c r="E20" s="61" t="s">
         <v>44</v>
       </c>
@@ -4552,10 +4547,10 @@
       </c>
     </row>
     <row r="21" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A21" s="103"/>
-      <c r="B21" s="96"/>
-      <c r="C21" s="125"/>
-      <c r="D21" s="96"/>
+      <c r="A21" s="100"/>
+      <c r="B21" s="103"/>
+      <c r="C21" s="106"/>
+      <c r="D21" s="103"/>
       <c r="E21" s="49" t="s">
         <v>46</v>
       </c>
@@ -4631,16 +4626,16 @@
       <c r="V22" s="25"/>
     </row>
     <row r="23" spans="1:22" s="25" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A23" s="101" t="s">
+      <c r="A23" s="98" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="116" t="s">
+      <c r="B23" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="116" t="s">
+      <c r="C23" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="94" t="s">
+      <c r="D23" s="101" t="s">
         <v>53</v>
       </c>
       <c r="E23" s="61" t="s">
@@ -4670,10 +4665,10 @@
       </c>
     </row>
     <row r="24" spans="1:22" s="25" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A24" s="102"/>
-      <c r="B24" s="116"/>
-      <c r="C24" s="116"/>
-      <c r="D24" s="95"/>
+      <c r="A24" s="99"/>
+      <c r="B24" s="107"/>
+      <c r="C24" s="107"/>
+      <c r="D24" s="102"/>
       <c r="E24" s="89" t="s">
         <v>56</v>
       </c>
@@ -4701,10 +4696,10 @@
       </c>
     </row>
     <row r="25" spans="1:22" ht="52.5" customHeight="1">
-      <c r="A25" s="102"/>
-      <c r="B25" s="116"/>
-      <c r="C25" s="116"/>
-      <c r="D25" s="95"/>
+      <c r="A25" s="99"/>
+      <c r="B25" s="107"/>
+      <c r="C25" s="107"/>
+      <c r="D25" s="102"/>
       <c r="E25" s="84" t="s">
         <v>36</v>
       </c>
@@ -4742,61 +4737,61 @@
       <c r="V25" s="25"/>
     </row>
     <row r="26" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A26" s="118" t="s">
+      <c r="A26" s="126" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="110" t="s">
+      <c r="B26" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="110" t="s">
+      <c r="C26" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="112" t="s">
+      <c r="D26" s="124" t="s">
         <v>61</v>
       </c>
       <c r="E26" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="110" t="s">
+      <c r="F26" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="97" t="s">
+      <c r="G26" s="136" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="109">
+      <c r="H26" s="134">
         <v>44012</v>
       </c>
-      <c r="I26" s="109">
+      <c r="I26" s="134">
         <v>44013</v>
       </c>
-      <c r="J26" s="112">
+      <c r="J26" s="124">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K26" s="111" t="s">
+      <c r="K26" s="135" t="s">
         <v>24</v>
       </c>
-      <c r="L26" s="104">
+      <c r="L26" s="129">
         <v>1</v>
       </c>
       <c r="M26" s="67"/>
       <c r="N26" s="48"/>
     </row>
     <row r="27" spans="1:22" ht="30" customHeight="1">
-      <c r="A27" s="119"/>
-      <c r="B27" s="110"/>
-      <c r="C27" s="110"/>
-      <c r="D27" s="113"/>
+      <c r="A27" s="127"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="128"/>
       <c r="E27" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="110"/>
-      <c r="G27" s="97"/>
-      <c r="H27" s="109"/>
-      <c r="I27" s="109"/>
-      <c r="J27" s="113"/>
-      <c r="K27" s="111"/>
-      <c r="L27" s="104"/>
+      <c r="F27" s="111"/>
+      <c r="G27" s="136"/>
+      <c r="H27" s="134"/>
+      <c r="I27" s="134"/>
+      <c r="J27" s="128"/>
+      <c r="K27" s="135"/>
+      <c r="L27" s="129"/>
       <c r="M27" s="67"/>
       <c r="N27" s="48"/>
       <c r="O27" s="25"/>
@@ -4809,16 +4804,16 @@
       <c r="V27" s="25"/>
     </row>
     <row r="28" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A28" s="101" t="s">
+      <c r="A28" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="110" t="s">
+      <c r="B28" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="110" t="s">
+      <c r="C28" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="110" t="s">
+      <c r="D28" s="111" t="s">
         <v>66</v>
       </c>
       <c r="E28" s="90" t="s">
@@ -4827,51 +4822,51 @@
       <c r="F28" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="97" t="s">
+      <c r="G28" s="136" t="s">
         <v>68</v>
       </c>
-      <c r="H28" s="108">
+      <c r="H28" s="133">
         <v>44010</v>
       </c>
-      <c r="I28" s="109">
+      <c r="I28" s="134">
         <v>44013</v>
       </c>
-      <c r="J28" s="110">
+      <c r="J28" s="111">
         <f>I28-H28</f>
         <v>3</v>
       </c>
-      <c r="K28" s="111" t="s">
+      <c r="K28" s="135" t="s">
         <v>24</v>
       </c>
-      <c r="L28" s="104">
+      <c r="L28" s="129">
         <v>1</v>
       </c>
       <c r="N28" s="48"/>
     </row>
     <row r="29" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A29" s="102"/>
-      <c r="B29" s="110"/>
-      <c r="C29" s="110"/>
-      <c r="D29" s="110"/>
+      <c r="A29" s="99"/>
+      <c r="B29" s="111"/>
+      <c r="C29" s="111"/>
+      <c r="D29" s="111"/>
       <c r="E29" s="92" t="s">
         <v>69</v>
       </c>
       <c r="F29" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="97"/>
-      <c r="H29" s="108"/>
-      <c r="I29" s="109"/>
-      <c r="J29" s="110"/>
-      <c r="K29" s="111"/>
-      <c r="L29" s="104"/>
+      <c r="G29" s="136"/>
+      <c r="H29" s="133"/>
+      <c r="I29" s="134"/>
+      <c r="J29" s="111"/>
+      <c r="K29" s="135"/>
+      <c r="L29" s="129"/>
       <c r="N29" s="48"/>
     </row>
     <row r="30" spans="1:22" ht="30" customHeight="1">
-      <c r="A30" s="103"/>
-      <c r="B30" s="110"/>
-      <c r="C30" s="110"/>
-      <c r="D30" s="110"/>
+      <c r="A30" s="100"/>
+      <c r="B30" s="111"/>
+      <c r="C30" s="111"/>
+      <c r="D30" s="111"/>
       <c r="E30" s="26" t="s">
         <v>70</v>
       </c>
@@ -4881,11 +4876,11 @@
       <c r="G30" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="H30" s="108"/>
-      <c r="I30" s="109"/>
-      <c r="J30" s="110"/>
-      <c r="K30" s="111"/>
-      <c r="L30" s="104"/>
+      <c r="H30" s="133"/>
+      <c r="I30" s="134"/>
+      <c r="J30" s="111"/>
+      <c r="K30" s="135"/>
+      <c r="L30" s="129"/>
       <c r="M30" s="25"/>
       <c r="N30" s="48"/>
       <c r="O30" s="25"/>
@@ -4898,16 +4893,16 @@
       <c r="V30" s="25"/>
     </row>
     <row r="31" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A31" s="101" t="s">
+      <c r="A31" s="98" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="94" t="s">
+      <c r="B31" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="123" t="s">
+      <c r="C31" s="104" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="94" t="s">
+      <c r="D31" s="101" t="s">
         <v>75</v>
       </c>
       <c r="E31" s="56" t="s">
@@ -4937,10 +4932,10 @@
       </c>
     </row>
     <row r="32" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A32" s="102"/>
-      <c r="B32" s="95"/>
-      <c r="C32" s="124"/>
-      <c r="D32" s="95"/>
+      <c r="A32" s="99"/>
+      <c r="B32" s="102"/>
+      <c r="C32" s="105"/>
+      <c r="D32" s="102"/>
       <c r="E32" s="44" t="s">
         <v>78</v>
       </c>
@@ -4967,10 +4962,10 @@
       </c>
     </row>
     <row r="33" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A33" s="102"/>
-      <c r="B33" s="95"/>
-      <c r="C33" s="124"/>
-      <c r="D33" s="95"/>
+      <c r="A33" s="99"/>
+      <c r="B33" s="102"/>
+      <c r="C33" s="105"/>
+      <c r="D33" s="102"/>
       <c r="E33" s="44" t="s">
         <v>80</v>
       </c>
@@ -4998,10 +4993,10 @@
       </c>
     </row>
     <row r="34" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A34" s="102"/>
-      <c r="B34" s="95"/>
-      <c r="C34" s="124"/>
-      <c r="D34" s="95"/>
+      <c r="A34" s="99"/>
+      <c r="B34" s="102"/>
+      <c r="C34" s="105"/>
+      <c r="D34" s="102"/>
       <c r="E34" s="44" t="s">
         <v>82</v>
       </c>
@@ -5029,10 +5024,10 @@
       </c>
     </row>
     <row r="35" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A35" s="102"/>
-      <c r="B35" s="95"/>
-      <c r="C35" s="124"/>
-      <c r="D35" s="95"/>
+      <c r="A35" s="99"/>
+      <c r="B35" s="102"/>
+      <c r="C35" s="105"/>
+      <c r="D35" s="102"/>
       <c r="E35" s="44" t="s">
         <v>84</v>
       </c>
@@ -5060,10 +5055,10 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="33" customHeight="1">
-      <c r="A36" s="103"/>
-      <c r="B36" s="96"/>
-      <c r="C36" s="125"/>
-      <c r="D36" s="96"/>
+      <c r="A36" s="100"/>
+      <c r="B36" s="103"/>
+      <c r="C36" s="106"/>
+      <c r="D36" s="103"/>
       <c r="E36" s="44" t="s">
         <v>86</v>
       </c>
@@ -5142,12 +5137,12 @@
       <c r="A38" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="98"/>
-      <c r="C38" s="99"/>
-      <c r="D38" s="99"/>
-      <c r="E38" s="99"/>
-      <c r="F38" s="99"/>
-      <c r="G38" s="100"/>
+      <c r="B38" s="137"/>
+      <c r="C38" s="138"/>
+      <c r="D38" s="138"/>
+      <c r="E38" s="138"/>
+      <c r="F38" s="138"/>
+      <c r="G38" s="139"/>
       <c r="H38" s="27">
         <v>43837</v>
       </c>
@@ -5176,14 +5171,14 @@
       <c r="V38" s="25"/>
     </row>
     <row r="39" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A39" s="94" t="s">
+      <c r="A39" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="94" t="s">
+      <c r="B39" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="94"/>
-      <c r="D39" s="94" t="s">
+      <c r="C39" s="101"/>
+      <c r="D39" s="101" t="s">
         <v>96</v>
       </c>
       <c r="E39" s="63" t="s">
@@ -5213,10 +5208,10 @@
       <c r="N39" s="48"/>
     </row>
     <row r="40" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A40" s="95"/>
-      <c r="B40" s="95"/>
-      <c r="C40" s="95"/>
-      <c r="D40" s="95"/>
+      <c r="A40" s="102"/>
+      <c r="B40" s="102"/>
+      <c r="C40" s="102"/>
+      <c r="D40" s="102"/>
       <c r="E40" s="49" t="s">
         <v>100</v>
       </c>
@@ -5244,10 +5239,10 @@
       <c r="N40" s="48"/>
     </row>
     <row r="41" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A41" s="95"/>
-      <c r="B41" s="95"/>
-      <c r="C41" s="95"/>
-      <c r="D41" s="95"/>
+      <c r="A41" s="102"/>
+      <c r="B41" s="102"/>
+      <c r="C41" s="102"/>
+      <c r="D41" s="102"/>
       <c r="E41" s="49" t="s">
         <v>102</v>
       </c>
@@ -5275,10 +5270,10 @@
       <c r="N41" s="48"/>
     </row>
     <row r="42" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A42" s="95"/>
-      <c r="B42" s="95"/>
-      <c r="C42" s="95"/>
-      <c r="D42" s="95"/>
+      <c r="A42" s="102"/>
+      <c r="B42" s="102"/>
+      <c r="C42" s="102"/>
+      <c r="D42" s="102"/>
       <c r="E42" s="63" t="s">
         <v>104</v>
       </c>
@@ -5306,10 +5301,10 @@
       <c r="N42" s="48"/>
     </row>
     <row r="43" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A43" s="96"/>
-      <c r="B43" s="96"/>
-      <c r="C43" s="96"/>
-      <c r="D43" s="96"/>
+      <c r="A43" s="103"/>
+      <c r="B43" s="103"/>
+      <c r="C43" s="103"/>
+      <c r="D43" s="103"/>
       <c r="E43" s="43" t="s">
         <v>106</v>
       </c>
@@ -5386,16 +5381,16 @@
       <c r="V44" s="25"/>
     </row>
     <row r="45" spans="1:22" s="25" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A45" s="101" t="s">
+      <c r="A45" s="98" t="s">
         <v>113</v>
       </c>
-      <c r="B45" s="94" t="s">
+      <c r="B45" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="123" t="s">
+      <c r="C45" s="104" t="s">
         <v>114</v>
       </c>
-      <c r="D45" s="101" t="s">
+      <c r="D45" s="98" t="s">
         <v>27</v>
       </c>
       <c r="E45" s="43" t="s">
@@ -5425,10 +5420,10 @@
       <c r="N45" s="48"/>
     </row>
     <row r="46" spans="1:22" ht="46.5" customHeight="1">
-      <c r="A46" s="103"/>
-      <c r="B46" s="96"/>
-      <c r="C46" s="125"/>
-      <c r="D46" s="103"/>
+      <c r="A46" s="100"/>
+      <c r="B46" s="103"/>
+      <c r="C46" s="106"/>
+      <c r="D46" s="100"/>
       <c r="E46" s="90" t="s">
         <v>117</v>
       </c>
@@ -5466,19 +5461,19 @@
       <c r="V46" s="25"/>
     </row>
     <row r="47" spans="1:22" ht="30.75" customHeight="1">
-      <c r="A47" s="131" t="s">
+      <c r="A47" s="97" t="s">
         <v>118</v>
       </c>
-      <c r="B47" s="131"/>
-      <c r="C47" s="131"/>
-      <c r="D47" s="131"/>
-      <c r="E47" s="131"/>
-      <c r="F47" s="131"/>
-      <c r="G47" s="131"/>
-      <c r="H47" s="131"/>
-      <c r="I47" s="131"/>
-      <c r="J47" s="131"/>
-      <c r="K47" s="131"/>
+      <c r="B47" s="97"/>
+      <c r="C47" s="97"/>
+      <c r="D47" s="97"/>
+      <c r="E47" s="97"/>
+      <c r="F47" s="97"/>
+      <c r="G47" s="97"/>
+      <c r="H47" s="97"/>
+      <c r="I47" s="97"/>
+      <c r="J47" s="97"/>
+      <c r="K47" s="97"/>
       <c r="L47" s="38"/>
       <c r="M47" s="25"/>
       <c r="N47" s="25"/>
@@ -5548,16 +5543,16 @@
       </c>
     </row>
     <row r="50" spans="1:22" ht="38.25" customHeight="1">
-      <c r="A50" s="126" t="s">
+      <c r="A50" s="120" t="s">
         <v>122</v>
       </c>
-      <c r="B50" s="110" t="s">
+      <c r="B50" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="123" t="s">
+      <c r="C50" s="104" t="s">
         <v>123</v>
       </c>
-      <c r="D50" s="128"/>
+      <c r="D50" s="108"/>
       <c r="E50" s="44" t="s">
         <v>124</v>
       </c>
@@ -5595,10 +5590,10 @@
       <c r="V50" s="25"/>
     </row>
     <row r="51" spans="1:22" s="25" customFormat="1" ht="45" customHeight="1">
-      <c r="A51" s="126"/>
-      <c r="B51" s="110"/>
-      <c r="C51" s="125"/>
-      <c r="D51" s="129"/>
+      <c r="A51" s="120"/>
+      <c r="B51" s="111"/>
+      <c r="C51" s="106"/>
+      <c r="D51" s="109"/>
       <c r="E51" s="49" t="s">
         <v>126</v>
       </c>
@@ -5626,16 +5621,16 @@
       </c>
     </row>
     <row r="52" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A52" s="130" t="s">
+      <c r="A52" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="B52" s="110" t="s">
+      <c r="B52" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="C52" s="116" t="s">
+      <c r="C52" s="107" t="s">
         <v>123</v>
       </c>
-      <c r="D52" s="110"/>
+      <c r="D52" s="111"/>
       <c r="E52" s="88" t="s">
         <v>129</v>
       </c>
@@ -5663,10 +5658,10 @@
       </c>
     </row>
     <row r="53" spans="1:22" s="25" customFormat="1" ht="57" customHeight="1">
-      <c r="A53" s="130"/>
-      <c r="B53" s="110"/>
-      <c r="C53" s="116"/>
-      <c r="D53" s="110"/>
+      <c r="A53" s="110"/>
+      <c r="B53" s="111"/>
+      <c r="C53" s="107"/>
+      <c r="D53" s="111"/>
       <c r="E53" s="88" t="s">
         <v>130</v>
       </c>
@@ -5694,16 +5689,16 @@
       </c>
     </row>
     <row r="54" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A54" s="126" t="s">
+      <c r="A54" s="120" t="s">
         <v>132</v>
       </c>
-      <c r="B54" s="127" t="s">
+      <c r="B54" s="121" t="s">
         <v>60</v>
       </c>
-      <c r="C54" s="116" t="s">
+      <c r="C54" s="107" t="s">
         <v>133</v>
       </c>
-      <c r="D54" s="127"/>
+      <c r="D54" s="121"/>
       <c r="E54" s="88" t="s">
         <v>134</v>
       </c>
@@ -5731,10 +5726,10 @@
       </c>
     </row>
     <row r="55" spans="1:22" s="25" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A55" s="126"/>
-      <c r="B55" s="127"/>
-      <c r="C55" s="116"/>
-      <c r="D55" s="127"/>
+      <c r="A55" s="120"/>
+      <c r="B55" s="121"/>
+      <c r="C55" s="107"/>
+      <c r="D55" s="121"/>
       <c r="E55" s="90" t="s">
         <v>136</v>
       </c>
@@ -5826,16 +5821,16 @@
       </c>
     </row>
     <row r="58" spans="1:22" s="25" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A58" s="120" t="s">
+      <c r="A58" s="117" t="s">
         <v>142</v>
       </c>
-      <c r="B58" s="94" t="s">
+      <c r="B58" s="101" t="s">
         <v>141</v>
       </c>
-      <c r="C58" s="123" t="s">
+      <c r="C58" s="104" t="s">
         <v>143</v>
       </c>
-      <c r="D58" s="94"/>
+      <c r="D58" s="101"/>
       <c r="E58" s="49" t="s">
         <v>144</v>
       </c>
@@ -5863,10 +5858,10 @@
       </c>
     </row>
     <row r="59" spans="1:22" s="25" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A59" s="121"/>
-      <c r="B59" s="95"/>
-      <c r="C59" s="124"/>
-      <c r="D59" s="95"/>
+      <c r="A59" s="118"/>
+      <c r="B59" s="102"/>
+      <c r="C59" s="105"/>
+      <c r="D59" s="102"/>
       <c r="E59" s="84" t="s">
         <v>146</v>
       </c>
@@ -5893,10 +5888,10 @@
       </c>
     </row>
     <row r="60" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A60" s="122"/>
-      <c r="B60" s="96"/>
-      <c r="C60" s="125"/>
-      <c r="D60" s="96"/>
+      <c r="A60" s="119"/>
+      <c r="B60" s="103"/>
+      <c r="C60" s="106"/>
+      <c r="D60" s="103"/>
       <c r="E60" s="84" t="s">
         <v>148</v>
       </c>
@@ -5921,16 +5916,16 @@
       </c>
     </row>
     <row r="61" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A61" s="130" t="s">
+      <c r="A61" s="110" t="s">
         <v>149</v>
       </c>
-      <c r="B61" s="94" t="s">
+      <c r="B61" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="C61" s="123" t="s">
+      <c r="C61" s="104" t="s">
         <v>150</v>
       </c>
-      <c r="D61" s="128"/>
+      <c r="D61" s="108"/>
       <c r="E61" s="61" t="s">
         <v>151</v>
       </c>
@@ -5958,10 +5953,10 @@
       </c>
     </row>
     <row r="62" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A62" s="130"/>
-      <c r="B62" s="95"/>
-      <c r="C62" s="124"/>
-      <c r="D62" s="135"/>
+      <c r="A62" s="110"/>
+      <c r="B62" s="102"/>
+      <c r="C62" s="105"/>
+      <c r="D62" s="115"/>
       <c r="E62" s="61" t="s">
         <v>154</v>
       </c>
@@ -5989,10 +5984,10 @@
       </c>
     </row>
     <row r="63" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A63" s="130"/>
-      <c r="B63" s="133"/>
-      <c r="C63" s="134"/>
-      <c r="D63" s="136"/>
+      <c r="A63" s="110"/>
+      <c r="B63" s="113"/>
+      <c r="C63" s="114"/>
+      <c r="D63" s="116"/>
       <c r="E63" s="61" t="s">
         <v>156</v>
       </c>
@@ -6020,19 +6015,19 @@
       </c>
     </row>
     <row r="64" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A64" s="132" t="s">
+      <c r="A64" s="112" t="s">
         <v>159</v>
       </c>
-      <c r="B64" s="132"/>
-      <c r="C64" s="132"/>
-      <c r="D64" s="132"/>
-      <c r="E64" s="132"/>
-      <c r="F64" s="132"/>
-      <c r="G64" s="132"/>
-      <c r="H64" s="132"/>
-      <c r="I64" s="132"/>
-      <c r="J64" s="132"/>
-      <c r="K64" s="132"/>
+      <c r="B64" s="112"/>
+      <c r="C64" s="112"/>
+      <c r="D64" s="112"/>
+      <c r="E64" s="112"/>
+      <c r="F64" s="112"/>
+      <c r="G64" s="112"/>
+      <c r="H64" s="112"/>
+      <c r="I64" s="112"/>
+      <c r="J64" s="112"/>
+      <c r="K64" s="112"/>
       <c r="L64" s="57"/>
       <c r="M64" s="25"/>
       <c r="N64" s="25"/>
@@ -6670,19 +6665,19 @@
       <c r="V83" s="25"/>
     </row>
     <row r="84" spans="1:22" ht="25.5" customHeight="1">
-      <c r="A84" s="131" t="s">
+      <c r="A84" s="97" t="s">
         <v>179</v>
       </c>
-      <c r="B84" s="131"/>
-      <c r="C84" s="131"/>
-      <c r="D84" s="131"/>
-      <c r="E84" s="131"/>
-      <c r="F84" s="131"/>
-      <c r="G84" s="131"/>
-      <c r="H84" s="131"/>
-      <c r="I84" s="131"/>
-      <c r="J84" s="131"/>
-      <c r="K84" s="131"/>
+      <c r="B84" s="97"/>
+      <c r="C84" s="97"/>
+      <c r="D84" s="97"/>
+      <c r="E84" s="97"/>
+      <c r="F84" s="97"/>
+      <c r="G84" s="97"/>
+      <c r="H84" s="97"/>
+      <c r="I84" s="97"/>
+      <c r="J84" s="97"/>
+      <c r="K84" s="97"/>
       <c r="L84" s="38"/>
       <c r="M84" s="25"/>
       <c r="N84" s="25"/>
@@ -6861,6 +6856,64 @@
     </row>
   </sheetData>
   <mergeCells count="74">
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="D39:D43"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="D31:D36"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="L28:L30"/>
+    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="D58:D60"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A84:K84"/>
+    <mergeCell ref="A64:K64"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="D61:D63"/>
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B4:H4"/>
@@ -6877,64 +6930,6 @@
     <mergeCell ref="A31:A36"/>
     <mergeCell ref="B31:B36"/>
     <mergeCell ref="C31:C36"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A84:K84"/>
-    <mergeCell ref="A64:K64"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="D61:D63"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="D58:D60"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="L28:L30"/>
-    <mergeCell ref="D13:D17"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="K28:K30"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="C39:C43"/>
-    <mergeCell ref="D39:D43"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="D31:D36"/>
-    <mergeCell ref="A28:A30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G20" r:id="rId1"/>

</xml_diff>